<commit_message>
user stories - clinic
</commit_message>
<xml_diff>
--- a/Analytics/VAC user stories.xlsx
+++ b/Analytics/VAC user stories.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
   <si>
     <t>Module</t>
   </si>
@@ -92,9 +92,6 @@
     <t>view my appointments and their statuses</t>
   </si>
   <si>
-    <t>I can view that my appointment is confirmed or not and when I should visit the clinic</t>
-  </si>
-  <si>
     <t>view my appointment details</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>other users can view clinic info</t>
   </si>
   <si>
-    <t>address, name</t>
-  </si>
-  <si>
     <t>log in to application with login and password</t>
   </si>
   <si>
@@ -153,6 +147,30 @@
   </si>
   <si>
     <t>patients can show the time, when I can make an appointment</t>
+  </si>
+  <si>
+    <t>I can view that my appointment is confirmed by me or not and when I should visit the clinic</t>
+  </si>
+  <si>
+    <t>confirm if vaccination took place</t>
+  </si>
+  <si>
+    <t>other process members can see if vaccination took place</t>
+  </si>
+  <si>
+    <t>view appointment details</t>
+  </si>
+  <si>
+    <t>I can clarify date and time of appointment</t>
+  </si>
+  <si>
+    <t>view patient info</t>
+  </si>
+  <si>
+    <t>I can get know which vaccination patient need</t>
+  </si>
+  <si>
+    <t>address, name, type, vacination types</t>
   </si>
 </sst>
 </file>
@@ -499,19 +517,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
@@ -599,7 +617,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -641,7 +659,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -652,10 +670,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -666,10 +684,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -680,13 +698,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -697,10 +715,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -711,46 +729,82 @@
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>42</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>